<commit_message>
Combined list with ICD10, OPCS4, and Read codes
Based on the codes from MOLL19 Supp Table1 but expanded and where possible OPCS4 were matched to Read codes as we noticed that procedures were recorded in GP data.
</commit_message>
<xml_diff>
--- a/0695-IIH/Diagnostic and procedure codes for IIH.xlsx
+++ b/0695-IIH/Diagnostic and procedure codes for IIH.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="222">
   <si>
     <t>Visual outcomes</t>
   </si>
@@ -176,15 +177,9 @@
     <t>H53.4</t>
   </si>
   <si>
-    <t>1B76.</t>
-  </si>
-  <si>
     <t>H53.8</t>
   </si>
   <si>
-    <t>XE16I</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gastroplasty NEC </t>
   </si>
   <si>
@@ -227,12 +222,6 @@
     <t xml:space="preserve">A12.4   </t>
   </si>
   <si>
-    <t>XE09j</t>
-  </si>
-  <si>
-    <t>XE09i</t>
-  </si>
-  <si>
     <t>Drainage of spinal canal</t>
   </si>
   <si>
@@ -260,15 +249,9 @@
     <t>Read Visual loss both eyes, unqualified gets mapped to Mild or no visual impairment in ICD10 (?)</t>
   </si>
   <si>
-    <t>Decompression of optic nerve</t>
-  </si>
-  <si>
     <t>A32.1</t>
   </si>
   <si>
-    <t>(optic nerve sheath fenestration)</t>
-  </si>
-  <si>
     <t>Obstetric History - used to see whether women with IIH had an increased risk of complex delivery</t>
   </si>
   <si>
@@ -324,13 +307,397 @@
   </si>
   <si>
     <t>R17</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>of</t>
+  </si>
+  <si>
+    <t>ventricle</t>
+  </si>
+  <si>
+    <t>brain</t>
+  </si>
+  <si>
+    <t>A12.1</t>
+  </si>
+  <si>
+    <t>Ventriculocisternostomy</t>
+  </si>
+  <si>
+    <t>A12.2</t>
+  </si>
+  <si>
+    <t>A12.3</t>
+  </si>
+  <si>
+    <t>A12.4</t>
+  </si>
+  <si>
+    <t>A12.5</t>
+  </si>
+  <si>
+    <t>A12.9</t>
+  </si>
+  <si>
+    <t>A13</t>
+  </si>
+  <si>
+    <t>A13.1</t>
+  </si>
+  <si>
+    <t>A13.2</t>
+  </si>
+  <si>
+    <t>A13.3</t>
+  </si>
+  <si>
+    <t>A13.4</t>
+  </si>
+  <si>
+    <t>A13.8</t>
+  </si>
+  <si>
+    <t>A13.9</t>
+  </si>
+  <si>
+    <t>A14</t>
+  </si>
+  <si>
+    <t>A14.1</t>
+  </si>
+  <si>
+    <t>A14.2</t>
+  </si>
+  <si>
+    <t>A14.3</t>
+  </si>
+  <si>
+    <t>A14.4</t>
+  </si>
+  <si>
+    <t>A14.5</t>
+  </si>
+  <si>
+    <t>A14.8</t>
+  </si>
+  <si>
+    <t>A14.9</t>
+  </si>
+  <si>
+    <t>A16</t>
+  </si>
+  <si>
+    <t>A16.1</t>
+  </si>
+  <si>
+    <t>A16.8</t>
+  </si>
+  <si>
+    <t>A16.9</t>
+  </si>
+  <si>
+    <t>A17</t>
+  </si>
+  <si>
+    <t>endoscopic</t>
+  </si>
+  <si>
+    <t>diagnostic</t>
+  </si>
+  <si>
+    <t>examination</t>
+  </si>
+  <si>
+    <t>(A18.9)</t>
+  </si>
+  <si>
+    <t>A52.1</t>
+  </si>
+  <si>
+    <t>A52.2</t>
+  </si>
+  <si>
+    <t>A52.3</t>
+  </si>
+  <si>
+    <t>A52.8</t>
+  </si>
+  <si>
+    <t>A52.9</t>
+  </si>
+  <si>
+    <t>A53</t>
+  </si>
+  <si>
+    <t>A53.1</t>
+  </si>
+  <si>
+    <t>A53.2</t>
+  </si>
+  <si>
+    <t>A53.3</t>
+  </si>
+  <si>
+    <t>A53.4</t>
+  </si>
+  <si>
+    <t>A53.5</t>
+  </si>
+  <si>
+    <t>A53.6</t>
+  </si>
+  <si>
+    <t>A53.8</t>
+  </si>
+  <si>
+    <t>A53.9</t>
+  </si>
+  <si>
+    <t>A54</t>
+  </si>
+  <si>
+    <t>A54.1</t>
+  </si>
+  <si>
+    <t>A54.2</t>
+  </si>
+  <si>
+    <t>A54.3</t>
+  </si>
+  <si>
+    <t>A54.4</t>
+  </si>
+  <si>
+    <t>A54.5</t>
+  </si>
+  <si>
+    <t>A54.8</t>
+  </si>
+  <si>
+    <t>A54.9</t>
+  </si>
+  <si>
+    <t>A55</t>
+  </si>
+  <si>
+    <t>A55.1</t>
+  </si>
+  <si>
+    <t>A55.2</t>
+  </si>
+  <si>
+    <t>A55.3</t>
+  </si>
+  <si>
+    <t>A55.8</t>
+  </si>
+  <si>
+    <t>A55.9</t>
+  </si>
+  <si>
+    <t>Creation of connection from ventricle of brain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creation of ventriculopleural shunt   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creation of ventriculoperitoneal shunt   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creation of subcutaneous cerebrospinal fluid reservoir </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other specified     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unspecified      </t>
+  </si>
+  <si>
+    <t>Attention to component of connection from ventricle</t>
+  </si>
+  <si>
+    <t>Maintenance of proximal catheter of cerebroventricular shunt</t>
+  </si>
+  <si>
+    <t>Maintenance of distal catheter of cerebroventricular shunt</t>
+  </si>
+  <si>
+    <t>Insertion of antisyphon device into cerebroventricular shunt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renewal of valve of cerebroventricular shunt </t>
+  </si>
+  <si>
+    <t>Other operations on connection from ventricle of brain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Renewal of cerebroventricular shunt    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Revision of cerebroventricular shunt NEC   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Includes: Conversion of cerebroventricular shunt NEC  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Removal of cerebroventricular shunt    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Irrigation of cerebroventricular shunt    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attention to cerebroventricular shunt NEC   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other specified      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unspecified       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other open operations on ventricle of brain </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open drainage of ventricle of brain NEC </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Therapeutic endoscopic operations on ventricle of brain </t>
+  </si>
+  <si>
+    <t>Note: It is not necessary to code additionally any mention of diagnostic endoscopic examination of ventricle of brain (A18.9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Therapeutic lumbar epidural injection    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Epidural blood patch     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drainage of spinal canal    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cerebrospinal syringostomy      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creation of thecoperitoneal shunt    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creation of syringoperitoneal shunt    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creation of lumboperitoneal shunt    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Drainage of cerebrospinal fluid NEC   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creation of lumbar subcutaneous shunt   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Therapeutic spinal puncture     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Injection of destructive substance into cerebrospinal fluid </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Injection of therapeutic substance into cerebrospinal fluid </t>
+  </si>
+  <si>
+    <t>Implantation of intrathecal drug delivery device adjacent to spinal cord</t>
+  </si>
+  <si>
+    <t>Attention to intrathecal drug delivery device adjacent to spinal cord</t>
+  </si>
+  <si>
+    <t>Removal of intrathecal drug delivery device adjacent to spinal cord</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagnostic spinal puncture     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radiculography       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spinal myelography NEC     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spinal manometry      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creation of ventriculovascular shunt   Includes: Creation of ventriculoatrial shunt  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Therapeutic sacral epidural injection   Includes: Caudal epidural     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unspecified       Includes: Lumbar puncture NEC    </t>
+  </si>
+  <si>
+    <t>Shunt complications (?)</t>
+  </si>
+  <si>
+    <t>Other - not certain how useful but we could check if there were any in our cohort - Owen to confirm.</t>
+  </si>
+  <si>
+    <t>Decompression of optic nerve (optic nerve sheath fenestration)</t>
+  </si>
+  <si>
+    <t>Not sure as subcodes (below) refer to injection but this one ?</t>
+  </si>
+  <si>
+    <t>F484.</t>
+  </si>
+  <si>
+    <t>F48y.</t>
+  </si>
+  <si>
+    <t>7010z</t>
+  </si>
+  <si>
+    <t>7010y</t>
+  </si>
+  <si>
+    <t>7011y</t>
+  </si>
+  <si>
+    <t>7011z</t>
+  </si>
+  <si>
+    <t>Revision of cerebroventricular shunt NEC   Includes: Conversion of cerebroventricular shunt NEC</t>
+  </si>
+  <si>
+    <t>7012y</t>
+  </si>
+  <si>
+    <t>7012z</t>
+  </si>
+  <si>
+    <t>7045y</t>
+  </si>
+  <si>
+    <t>7045z</t>
+  </si>
+  <si>
+    <t>Diagnostic spinal puncture</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -372,6 +739,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -393,7 +798,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -412,12 +817,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -699,18 +1112,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J57"/>
+  <dimension ref="A1:J123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="59" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="38.28515625" customWidth="1"/>
+    <col min="4" max="4" width="41.7109375" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" customWidth="1"/>
   </cols>
@@ -746,17 +1159,17 @@
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="15" t="s">
         <v>25</v>
       </c>
       <c r="D3" s="3"/>
-      <c r="E3" t="s">
+      <c r="E3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="15" t="s">
         <v>25</v>
       </c>
       <c r="G3" s="1"/>
@@ -835,7 +1248,7 @@
         <v>37</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -898,10 +1311,10 @@
         <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -912,230 +1325,1456 @@
         <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>2</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="11" t="s">
         <v>3</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="C22">
+        <v>76130</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+      <c r="C23">
+        <v>76131</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>4</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="11" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" t="s">
-        <v>68</v>
+        <v>60</v>
+      </c>
+      <c r="C29">
+        <v>70105</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="8">
+        <v>62</v>
+      </c>
+      <c r="C30">
         <v>70102</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31">
+        <v>70103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B33" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33">
+        <v>7010</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34">
+        <v>70100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B35" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35">
+        <v>70104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="B36" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>65</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B38" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38">
+        <v>7045</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>66</v>
       </c>
-      <c r="C31" t="s">
+      <c r="B39" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="9" t="s">
+      <c r="C39">
+        <v>70453</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40">
+        <v>70455</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="B42" t="s">
+        <v>136</v>
+      </c>
+      <c r="C42">
+        <v>70450</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="B43" t="s">
+        <v>137</v>
+      </c>
+      <c r="C43">
+        <v>70451</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B44" t="s">
+        <v>138</v>
+      </c>
+      <c r="C44">
+        <v>70452</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B45" t="s">
+        <v>140</v>
+      </c>
+      <c r="C45">
+        <v>70454</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B46" t="s">
+        <v>142</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="B47" t="s">
+        <v>143</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="8" t="s">
+        <v>193</v>
+      </c>
+      <c r="B49" t="s">
+        <v>144</v>
+      </c>
+      <c r="C49">
+        <v>7046</v>
+      </c>
+      <c r="D49" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B50" t="s">
+        <v>152</v>
+      </c>
+      <c r="C50">
+        <v>7047</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="B51" t="s">
+        <v>74</v>
+      </c>
+      <c r="C51">
+        <v>70280</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="8"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="10" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>165</v>
+      </c>
+      <c r="B55" t="s">
+        <v>106</v>
+      </c>
+      <c r="C55">
+        <v>7011</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>166</v>
+      </c>
+      <c r="B57" t="s">
+        <v>107</v>
+      </c>
+      <c r="C57">
+        <v>70110</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>167</v>
+      </c>
+      <c r="B58" t="s">
+        <v>108</v>
+      </c>
+      <c r="C58">
+        <v>70111</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>168</v>
+      </c>
+      <c r="B59" t="s">
+        <v>109</v>
+      </c>
+      <c r="C59">
+        <v>70112</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>169</v>
+      </c>
+      <c r="B60" t="s">
+        <v>110</v>
+      </c>
+      <c r="C60">
+        <v>70114</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>163</v>
+      </c>
+      <c r="B61" t="s">
+        <v>111</v>
+      </c>
+      <c r="C61" s="16" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>164</v>
+      </c>
+      <c r="B62" t="s">
+        <v>112</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>170</v>
+      </c>
+      <c r="B64" t="s">
+        <v>113</v>
+      </c>
+      <c r="C64">
+        <v>7012</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>172</v>
+      </c>
+      <c r="B65" t="s">
+        <v>114</v>
+      </c>
+      <c r="C65">
+        <v>70123</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>216</v>
+      </c>
+      <c r="B66" t="s">
+        <v>115</v>
+      </c>
+      <c r="C66">
+        <v>70124</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>175</v>
+      </c>
+      <c r="B67" t="s">
+        <v>116</v>
+      </c>
+      <c r="C67">
+        <v>70121</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>176</v>
+      </c>
+      <c r="B68" t="s">
+        <v>117</v>
+      </c>
+      <c r="C68">
+        <v>70120</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>177</v>
+      </c>
+      <c r="B69" t="s">
+        <v>118</v>
+      </c>
+      <c r="C69">
+        <v>70125</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>178</v>
+      </c>
+      <c r="B70" t="s">
+        <v>119</v>
+      </c>
+      <c r="C70" s="16" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>179</v>
+      </c>
+      <c r="B71" t="s">
+        <v>120</v>
+      </c>
+      <c r="C71" s="16" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B32" t="s">
+    </row>
+    <row r="79" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B79" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>69</v>
-      </c>
-      <c r="B35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35">
-        <v>7045</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>70</v>
-      </c>
-      <c r="B36" t="s">
-        <v>71</v>
-      </c>
-      <c r="C36">
-        <v>70453</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>73</v>
-      </c>
-      <c r="B37" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="s">
+      <c r="B80" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B81" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>88</v>
+      </c>
+      <c r="B82" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>92</v>
+      </c>
+      <c r="B83" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>90</v>
+      </c>
+      <c r="B84" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>77</v>
+      </c>
+      <c r="B85" t="s">
         <v>78</v>
       </c>
-      <c r="B39" t="s">
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
+      <c r="B86" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="10" t="s">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="B87" t="s">
         <v>82</v>
       </c>
-      <c r="B46" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>94</v>
-      </c>
-      <c r="B50" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>98</v>
-      </c>
-      <c r="B51" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>96</v>
-      </c>
-      <c r="B52" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>83</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B88" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>85</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B89" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>87</v>
-      </c>
-      <c r="B55" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>89</v>
-      </c>
-      <c r="B56" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>91</v>
-      </c>
-      <c r="B57" t="s">
-        <v>92</v>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A94" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="B94" s="14"/>
+      <c r="C94" s="14"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>180</v>
+      </c>
+      <c r="B96" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>181</v>
+      </c>
+      <c r="B97" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>178</v>
+      </c>
+      <c r="B98" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>179</v>
+      </c>
+      <c r="B99" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>182</v>
+      </c>
+      <c r="B102" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>184</v>
+      </c>
+      <c r="B104" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>204</v>
+      </c>
+      <c r="B105" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>185</v>
+      </c>
+      <c r="B106" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>178</v>
+      </c>
+      <c r="B107" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>179</v>
+      </c>
+      <c r="B108" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>194</v>
+      </c>
+      <c r="B110" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>195</v>
+      </c>
+      <c r="B111" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>196</v>
+      </c>
+      <c r="B112" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>197</v>
+      </c>
+      <c r="B113" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>198</v>
+      </c>
+      <c r="B114" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>178</v>
+      </c>
+      <c r="B115" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>179</v>
+      </c>
+      <c r="B116" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>200</v>
+      </c>
+      <c r="B119" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>201</v>
+      </c>
+      <c r="B120" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>202</v>
+      </c>
+      <c r="B121" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>178</v>
+      </c>
+      <c r="B122" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>205</v>
+      </c>
+      <c r="B123" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T95"/>
+  <sheetViews>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="B88" sqref="B88"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="56" customWidth="1"/>
+    <col min="3" max="9" width="43.42578125" customWidth="1"/>
+    <col min="10" max="10" width="121.7109375" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" customWidth="1"/>
+    <col min="12" max="12" width="6.85546875" hidden="1" customWidth="1"/>
+    <col min="13" max="15" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="1.85546875" customWidth="1"/>
+    <col min="17" max="20" width="9.140625" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B17" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>109</v>
+      </c>
+      <c r="B18" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>110</v>
+      </c>
+      <c r="B19" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>112</v>
+      </c>
+      <c r="B21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>114</v>
+      </c>
+      <c r="B25" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>116</v>
+      </c>
+      <c r="B30" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>117</v>
+      </c>
+      <c r="B31" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>119</v>
+      </c>
+      <c r="B33" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>120</v>
+      </c>
+      <c r="B34" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>121</v>
+      </c>
+      <c r="B36" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>123</v>
+      </c>
+      <c r="B39" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>125</v>
+      </c>
+      <c r="B42" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>183</v>
+      </c>
+      <c r="L43" t="s">
+        <v>96</v>
+      </c>
+      <c r="M43" t="s">
+        <v>127</v>
+      </c>
+      <c r="N43" t="s">
+        <v>126</v>
+      </c>
+      <c r="O43" t="s">
+        <v>128</v>
+      </c>
+      <c r="P43" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>97</v>
+      </c>
+      <c r="R43" t="s">
+        <v>96</v>
+      </c>
+      <c r="S43" t="s">
+        <v>98</v>
+      </c>
+      <c r="T43" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>130</v>
+      </c>
+      <c r="B44" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>131</v>
+      </c>
+      <c r="B45" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>132</v>
+      </c>
+      <c r="B49" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>133</v>
+      </c>
+      <c r="B50" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>134</v>
+      </c>
+      <c r="B51" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>135</v>
+      </c>
+      <c r="B53" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>136</v>
+      </c>
+      <c r="B55" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>137</v>
+      </c>
+      <c r="B56" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>138</v>
+      </c>
+      <c r="B57" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>139</v>
+      </c>
+      <c r="B58" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>140</v>
+      </c>
+      <c r="B59" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>141</v>
+      </c>
+      <c r="B60" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>142</v>
+      </c>
+      <c r="B61" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>143</v>
+      </c>
+      <c r="B62" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>144</v>
+      </c>
+      <c r="B64" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>145</v>
+      </c>
+      <c r="B66" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>146</v>
+      </c>
+      <c r="B67" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>147</v>
+      </c>
+      <c r="B68" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>148</v>
+      </c>
+      <c r="B69" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>149</v>
+      </c>
+      <c r="B70" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>150</v>
+      </c>
+      <c r="B71" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>151</v>
+      </c>
+      <c r="B72" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>152</v>
+      </c>
+      <c r="B74" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>153</v>
+      </c>
+      <c r="B76" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>154</v>
+      </c>
+      <c r="B77" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>155</v>
+      </c>
+      <c r="B78" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>157</v>
+      </c>
+      <c r="B80" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>171</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>